<commit_message>
add : city and location
</commit_message>
<xml_diff>
--- a/filtered_companies.xlsx
+++ b/filtered_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10xConstruction.ai - Mechanical</t>
+          <t>1Clicktech Global Services Pvt. Ltd.,Gurugram</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -467,67 +467,67 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Gurgaon</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10xConstruction.ai - Robotics</t>
+          <t>Aditya Birla Science &amp; Technology Company Ltd. (ABSTC) ,Mumbai</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Chemical</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1Clicktech Global Services Pvt. Ltd.,Gurugram</t>
+          <t>AECOM - Pune</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Gurgaon</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Aditya Birla Science &amp; Technology Company Ltd. (ABSTC) ,Mumbai</t>
+          <t>AECOM,Mumbai</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Chemical</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -700,27 +700,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CNH Industrial (India) Pvt. Ltd</t>
+          <t>CodeRound - Non Tech</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Noida</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CodeRound - Non Tech</t>
+          <t>CodeRound - Tech</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>25000</v>
+        <v>40000</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -740,36 +740,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CodeRound - Tech</t>
+          <t>Complete lnstrumentation Solutions Pvt. Ltd.,Gurugram</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Gurgaon</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Complete lnstrumentation Solutions Pvt. Ltd.,Gurugram</t>
+          <t>Critical Path Technologies Private Limited (“SalarySe) - Product</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Infrastructure</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>61000</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -780,32 +780,32 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Critical Path Technologies Private Limited (“SalarySe) - Product</t>
+          <t>CSIR - National chemical laboratory, Pune</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Chemical</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>61000</v>
+        <v>0</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Gurgaon</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CSIR - National chemical laboratory, Pune</t>
+          <t>CSIR NML</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Chemical</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -813,19 +813,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Jamshedpur</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CSIR NML</t>
+          <t>CSIR-NAL</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -833,19 +833,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Jamshedpur</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CSIR-NAL</t>
+          <t>DMI Finance Limited</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -853,14 +853,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>New Delhi</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DMI Finance Limited</t>
+          <t>Dunboxed Solutions Private Limited</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -869,11 +869,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>New Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Dunboxed Solutions Private Limited</t>
+          <t>e6data,Bengaluru</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -949,18 +949,18 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>e6data,Bengaluru</t>
+          <t>ENEA, Hyderabad</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -973,14 +973,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ENEA, Hyderabad</t>
+          <t>Engati Technologies Private Limited - Data Science</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -989,18 +989,18 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Engati Technologies Private Limited - Data Science</t>
+          <t>Engati Technologies Private Limited - Product Management</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>50000</v>
+        <v>45000</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1020,16 +1020,16 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Engati Technologies Private Limited - Product Management</t>
+          <t>Ennoventure Bengaluru</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>45000</v>
+        <v>0</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1040,16 +1040,16 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ennoventure Bengaluru</t>
+          <t>Eureka Forbes Ltd - Chemical</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>Chemical</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1060,12 +1060,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Eureka Forbes Ltd - Chemical</t>
+          <t>Eureka Forbes Ltd - Data Analytics</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Chemical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1073,14 +1073,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Eureka Forbes Ltd - Data Analytics</t>
+          <t>Eureka Forbes Ltd - Embedded Systems</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1093,19 +1093,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Eureka Forbes Ltd - Embedded Systems</t>
+          <t>Eureka Forbes Ltd - Mechanical</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Chemical</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1120,56 +1120,56 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Eureka Forbes Ltd - Mechanical</t>
+          <t>Exobot Dynamics Pvt Ltd,Sonepat</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Chemical</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Sonipat</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Exobot Dynamics Pvt Ltd,Sonepat</t>
+          <t>FemtoWeb Technologies Pvt Ltd ( Nanonets )</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Sonipat</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>FemtoWeb Technologies Pvt Ltd ( Nanonets )</t>
+          <t>Frontier Tower Associates Philippines Inc.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1180,16 +1180,16 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Frontier Tower Associates Philippines Inc.</t>
+          <t>Giga Health - Healthcare</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1200,7 +1200,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Giga Health - Healthcare</t>
+          <t>Giga Health - Product</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1220,65 +1220,65 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Giga Health - Product</t>
+          <t>Goldman Sachs - Hyderabad</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Goldman Sachs - Hyderabad</t>
+          <t>Goodera  - Software Development Engineer Testing  (SDET)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Infrastructure</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
+          <t>Finance and Mgmt</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Goodera  - Software Development Engineer Testing  (SDET)</t>
+          <t>Grasim Industries Ltd - Pulp &amp; Fibre Business - CRM, Mumbai</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr"/>
+          <t>Mechanical</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Grasim Industries Ltd - Pulp &amp; Fibre Business - CRM, Mumbai</t>
+          <t>Grasim Industries,Nagda</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1291,94 +1291,94 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Nagda</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Grasim Industries,Nagda</t>
+          <t>HEX Advisory Group, Gurgaon</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Nagda</t>
+          <t>Gurgaon</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GreenFortune Windows and Doors - Business Analytics.</t>
+          <t>HEX Advisory Group, Gurgaon</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Infrastructure</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>40000</v>
+        <v>25000</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Gurgaon</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>GreenFortune Windows and Doors - Product Strategy</t>
+          <t>Indian Institute of Petroleum ( IIP ),Dehradun</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Infrastructure</t>
+          <t>Chemical</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Dehradun</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>HEX Advisory Group, Gurgaon</t>
+          <t>Integrated Active Monitoring Pvt. Ltd.,Pune</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Gurgaon</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>HEX Advisory Group, Gurgaon</t>
+          <t>InterviewVector - Sales Development (Domestic)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1398,27 +1398,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>IAMSTILLALIVE ONCO ECOSYSTEM PVT LTD</t>
+          <t>InterviewVector - Sales Development (US)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Kolhapur</t>
+          <t>Gurgaon</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>IFB Industries,Goa</t>
+          <t>ITC Limited, PSPD - Tribeni (Kolkata)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1431,19 +1431,19 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Goa</t>
+          <t>Kolkata</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Indian Institute of Petroleum ( IIP ),Dehradun</t>
+          <t>ITC Limited, PSPD (Paperboards and Specialty Papers Division), Bhadrachalam</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Chemical</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1451,52 +1451,54 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Dehradun</t>
+          <t>Bhadrachalam</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>InMobi Technologies Pvt Ltd -  Business/ Product Analytics</t>
+          <t>JPMC - Chief Data &amp; Analytics Office</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
+          <t>Finance and Mgmt</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>150000</v>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Integrated Active Monitoring Pvt. Ltd.,Pune</t>
+          <t>JPMC - CIB R&amp;A - Banking</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>InterviewVector - Sales Development (Domestic)</t>
+          <t>JPMC - CIB R&amp;A – Global Research</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1505,18 +1507,18 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>25000</v>
+        <v>150000</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Gurgaon</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>InterviewVector - Sales Development (US)</t>
+          <t>JPMC - CIB R&amp;A – Markets – Sales &amp; CCAR</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1525,58 +1527,58 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>25000</v>
+        <v>150000</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Gurgaon</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ITC Limited, PSPD - Tribeni (Kolkata)</t>
+          <t>JPMC - CIB Research &amp; Analytics,Research Modernization – Project Management</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Kolkata</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ITC Limited, PSPD (Paperboards and Specialty Papers Division), Bhadrachalam</t>
+          <t>JPMC - GR&amp;C - CCB Risk Strategic Analytics</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Bhadrachalam</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>JPMC - Chief Data &amp; Analytics Office</t>
+          <t>JPMC - GR&amp;C –Model Risk Governance &amp; Review (MRGR) Quantitative Analytics</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1596,7 +1598,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>JPMC - CIB R&amp;A - Banking</t>
+          <t>JPMC - GR&amp;C WCR Counterparty Credit Risk</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1616,7 +1618,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>JPMC - CIB R&amp;A – Global Research</t>
+          <t>JPMC - GR&amp;C WCR Portfolio Analytics - Risk Grading Methodology &amp; Climate Risk</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1636,7 +1638,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>JPMC - CIB R&amp;A – Markets – Sales &amp; CCAR</t>
+          <t>JPMC - GR&amp;C WCR Portfolio Analytics- Analytics Strategy</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1656,7 +1658,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>JPMC - CIB Research &amp; Analytics,Research Modernization – Project Management</t>
+          <t>JPMC - Markets – Sales &amp; CCAR</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1676,7 +1678,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>JPMC - GR&amp;C - CCB Risk Strategic Analytics</t>
+          <t>JPMC - Markets - Trading &amp; Structuring</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1696,7 +1698,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>JPMC - GR&amp;C –Model Risk Governance &amp; Review (MRGR) Quantitative Analytics</t>
+          <t>JPMC - Risk Reporting &amp; Middle Office/Risk Controller</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1716,76 +1718,76 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>JPMC - GR&amp;C WCR Counterparty Credit Risk</t>
+          <t>Konecranes &amp; Demag Pvt Ltd</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>150000</v>
+        <v>20000</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>JPMC - GR&amp;C WCR Portfolio Analytics - Risk Grading Methodology &amp; Climate Risk</t>
+          <t>Longstraw Carbon Pvt. Ltd</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>150000</v>
+        <v>8000</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>JPMC - GR&amp;C WCR Portfolio Analytics- Analytics Strategy</t>
+          <t>Mahindra Accelo Ltd- Chakan (Pune)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>JPMC - Markets – Sales &amp; CCAR</t>
+          <t>Mahindra Accelo Ltd- Mumbai (Worli)</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1796,47 +1798,47 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>JPMC - Markets - Trading &amp; Structuring</t>
+          <t>MBB Labs Private Limited (Maybank),Bengaluru</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>150000</v>
+        <v>25000</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>JPMC - Risk Reporting &amp; Middle Office/Risk Controller</t>
+          <t>MELSS</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Chennai</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Mahindra Accelo Ltd- Chakan (Pune)</t>
+          <t>Mettler Toledo India Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1845,23 +1847,23 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Mahindra Accelo Ltd- Mumbai (Worli)</t>
+          <t>MIPS Embedded Technologies Pvt. Ltd,Bengaluru</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1869,63 +1871,63 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MBB Labs Private Limited (Maybank),Bengaluru</t>
+          <t>Morgan Stanley - IAD Data Analytics role</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>25000</v>
+        <v>100000</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MELSS</t>
+          <t>Morgan Stanley - IED GMG FE role</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Chennai</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Mettler Toledo India Pvt. Ltd.</t>
+          <t>Morgan Stanley FID - Counterparty Risk role</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1936,27 +1938,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MIPS Embedded Technologies Pvt. Ltd,Bengaluru</t>
+          <t>Morgan Stanley FID Research roles</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Morgan Stanley - IAD Data Analytics role</t>
+          <t>Morgan Stanley Primary Market Research role</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1965,7 +1967,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>100000</v>
+        <v>113000</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -1976,7 +1978,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Morgan Stanley - IED GMG FE role</t>
+          <t>Morgan Stanley-Funds Services Division - Client Computing Solutions</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1985,7 +1987,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>125000</v>
+        <v>113000</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -1996,7 +1998,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Morgan Stanley FID - Counterparty Risk role</t>
+          <t>Morgan Stanley-Funds Services Division - Portfolio Analytics</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2005,7 +2007,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>100000</v>
+        <v>113000</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2016,7 +2018,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Morgan Stanley FID Research roles</t>
+          <t>Morningstar - Index Management and Analytics,Mumbai</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2025,7 +2027,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>125000</v>
+        <v>0</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2036,27 +2038,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Morgan Stanley Primary Market Research role</t>
+          <t>National Centre for Biological Sciences (NCBS) ,Bengaluru</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>113000</v>
+        <v>0</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Morgan Stanley-Funds Services Division - Client Computing Solutions</t>
+          <t>NAVATA ROAD TRANSPORT</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2065,18 +2067,18 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>113000</v>
+        <v>0</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Morgan Stanley-Funds Services Division - Portfolio Analytics</t>
+          <t>NAVATA SUPPLY CHAIN SOLUTIONS PVT LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2085,58 +2087,58 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>113000</v>
+        <v>0</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Morningstar - Index Management and Analytics,Mumbai</t>
+          <t>Neurofin AI technologies Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>National Centre for Biological Sciences (NCBS) ,Bengaluru</t>
+          <t>Nirmaan Organization - Non Tech</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>NAVATA ROAD TRANSPORT</t>
+          <t>Novel Jewels – Aditya Birla Jewellery - Project / Infrastructure</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2145,138 +2147,138 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Mumbai</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>NAVATA SUPPLY CHAIN SOLUTIONS PVT LTD</t>
+          <t>Nutanix , Bengaluru</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>140000</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Necessa Security &amp; Integrated Services Pvt Ltd - Non Tech</t>
+          <t>Nvidia Graphics - Bengaluru</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Gurgaon</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Neurofin AI technologies Pvt. Ltd.</t>
+          <t>Pannaiamman&amp;Co</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Chennai</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Nirmaan Organization - Non Tech</t>
+          <t>Pioneer Electrocables Pvt Ltd</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Biratnagar, Morang, Nepal</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Norquest Brands Private Limited</t>
+          <t>Piramal Group - Tech, Bengaluru</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Novel Jewels – Aditya Birla Jewellery - Retail</t>
+          <t>Praj Industries</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Novel Jewels – Aditya Birla Jewellery - Supply Chain</t>
+          <t>Quickverse India Private Limited</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2285,47 +2287,47 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Aurangabad</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Novus Hi-Tech Robotic Systemz Pvt. Ltd.</t>
+          <t>Rainbow children’s Medicare Limited</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Gurgaon</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Novus Hi-Tech Robotic Systemz Pvt. Ltd.</t>
+          <t>Ramboll India Pvt Ltd</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2336,32 +2338,32 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Nutanix , Bengaluru</t>
+          <t>Ratham - Non Tech</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>140000</v>
+        <v>25000</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Nvidia Graphics - Bengaluru</t>
+          <t>Renesas, Bengaluru</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -2376,32 +2378,32 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Pioneer Electrocables Pvt Ltd</t>
+          <t>RISA Labs, Inc - Healthcare -Product</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Health Care</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Biratnagar, Morang, Nepal</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Piramal Group - Tech, Bengaluru</t>
+          <t>Rivos Systems - Bengaluru</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2416,12 +2418,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Praj Industries</t>
+          <t>RT Vision Technologies Pvt. Ltd</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2429,83 +2431,83 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Greater Noida</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Quickverse India Private Limited</t>
+          <t>Sarda Metals &amp; Alloys Ltd</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Aurangabad</t>
+          <t>Vizianagaram</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Rainbow children’s Medicare Limited</t>
+          <t>Sarvam AI - Backend engineering</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Ratham - Non Tech</t>
+          <t>Sarvam AI - Gen AI</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Infrastructure</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>25000</v>
+        <v>60000</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Renesas, Bengaluru</t>
+          <t>Sarvam AI - Gen AI</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -2516,16 +2518,16 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>RISA Labs, Inc - Healthcare -Product</t>
+          <t>Sarvam AI - GTM - Strategy</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Health Care</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -2536,16 +2538,16 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Rivos Systems - Bengaluru</t>
+          <t>Sarvam AI - ML</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2556,12 +2558,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>RT Vision Technologies Pvt. Ltd</t>
+          <t>Scapia Technology Private Limited</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2569,19 +2571,19 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Greater Noida</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Sarda Metals &amp; Alloys Ltd</t>
+          <t>ServCrust Private Limited, Hyderabad</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2589,23 +2591,23 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Vizianagaram</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Sarvam AI - Backend engineering</t>
+          <t>SG Analytics, Bengaluru</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -2616,16 +2618,16 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Sarvam AI - Gen AI</t>
+          <t>Shell India Markets Pvt. Ltd.,Bengaluru</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Chemical</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>60000</v>
+        <v>15000</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -2636,7 +2638,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Sarvam AI - Gen AI</t>
+          <t>SHVND Private Limited</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2645,18 +2647,18 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Secunderabad</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Sarvam AI - GTM - Strategy</t>
+          <t>Spanda.AI, Hyderabad</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2665,47 +2667,47 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Sarvam AI - ML</t>
+          <t>ST Microelectronics</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Electronics</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Noida</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Scapia Technology Private Limited</t>
+          <t>Stampmyvisa- IT</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -2716,7 +2718,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>ServCrust Private Limited, Hyderabad</t>
+          <t>Stampmyvisa- IT</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2725,23 +2727,23 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>SG Analytics, Bengaluru</t>
+          <t>Supra Sciences Private Llmited, Hyderabad</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Chemical</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2749,23 +2751,23 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Shell India Markets Pvt. Ltd.,Bengaluru</t>
+          <t>Swiss Re Global Business Solutions India Private Limited</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Chemical</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>15000</v>
+        <v>50000</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -2776,7 +2778,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>SHVND Private Limited</t>
+          <t>Synergiz Global Services Pvt Ltd</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2785,23 +2787,23 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Secunderabad</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Spanda.AI, Hyderabad</t>
+          <t>Tega Industries - Samali</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -2809,34 +2811,34 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Samali</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>ST Microelectronics</t>
+          <t>Telus AI - Product Management</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Noida</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Stampmyvisa- IT</t>
+          <t>TELUS AI- Product Designer</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2845,7 +2847,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>65000</v>
+        <v>45000</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -2856,7 +2858,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Stampmyvisa- IT</t>
+          <t>THINKBYTE TECHNOLOGIES PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2865,23 +2867,23 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>65000</v>
+        <v>15000</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Vijayawada</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Supra Sciences Private Llmited, Hyderabad</t>
+          <t>Thyssenkrupp Pune</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Chemical</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2889,74 +2891,74 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Pune</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Swiss Re Global Business Solutions India Private Limited</t>
+          <t>Timble Technologies</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>New Delhi</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Synergiz Global Services Pvt Ltd</t>
+          <t>Time tooth Technologies Pvt Ltd, Noida/Bengaluru</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Noida</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Tega Industries - Samali</t>
+          <t>Triomics Healthcare Pvt. Ltd- Product Management</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Samali</t>
+          <t>Bangalore</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Telus AI - Product Management</t>
+          <t>UBER - Bengaluru</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -2965,23 +2967,23 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Bangalore</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>TELUS AI- Product Designer</t>
+          <t>Udaan</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2996,12 +2998,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Texas Instruments -- Digital</t>
+          <t>Unity Growth Investments Pvt Ltd- Non Tech</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>Finance and Mgmt</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -3009,14 +3011,14 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>THINKBYTE TECHNOLOGIES PRIVATE LIMITED</t>
+          <t>Universal Software</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3025,38 +3027,38 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Vijayawada</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Thyssenkrupp Pune</t>
+          <t>Universal Software</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Timble Technologies</t>
+          <t>UST, Thiruvananthapuram</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3065,58 +3067,58 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>New Delhi</t>
+          <t>Thiruvananthapuram</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Time tooth Technologies Pvt Ltd, Noida/Bengaluru</t>
+          <t>UST, Thiruvananthapuram</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Noida</t>
+          <t>Thiruvananthapuram</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Triomics Healthcare Pvt. Ltd- Product Management</t>
+          <t>Virgio - Gen AI</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>UBER - Bengaluru</t>
+          <t>Virgio - UI Engineering</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3125,48 +3127,46 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Bengaluru</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Udaan</t>
+          <t>Virtuoso Optoelectronics Ltd - Packaging &amp; Product Design</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>45000</v>
+        <v>25000</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Nashik</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Unity Growth Investments Pvt Ltd- Non Tech</t>
+          <t>WILP - ADAS /  Autonomous Vehicle, Hyderabad</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Finance and Mgmt</t>
-        </is>
-      </c>
-      <c r="C137" t="n">
-        <v>0</v>
-      </c>
+          <t>Mechanical</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr"/>
       <c r="D137" t="inlineStr">
         <is>
           <t>Hyderabad</t>
@@ -3176,67 +3176,67 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Universal Software</t>
+          <t>WILP - Additive Manufacturing, Hyderabad</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>UST, Thiruvananthapuram</t>
+          <t>WILP - Electric and Hybrid Lab</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Thiruvananthapuram</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>UST, Thiruvananthapuram</t>
+          <t>WILP- Intelligent systems Lab</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Thiruvananthapuram</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Virgio - Gen AI</t>
+          <t>WILP, Hyderabad</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3245,347 +3245,129 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Virgio - UI Engineering</t>
+          <t>WILP-New Automotive Competency Centre Chennai (ACC)</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>CSIS/IT</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Bengaluru</t>
+          <t>Chennai</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Virtuoso Optoelectronics Ltd - Manufacturing</t>
+          <t>WILP-Vehicle security penetration testing facility in collaboration with Bosch</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>Mechanical</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Nashik</t>
+          <t>Hyderabad</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Virtuoso Optoelectronics Ltd - Packaging &amp; Product Design</t>
+          <t>Zeo - Product Content</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Nashik</t>
+          <t>Delaware</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Virtuoso Optoelectronics Ltd - Supply Chain &amp; Analytics</t>
+          <t>Zeo - Product Growth</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Nashik</t>
+          <t>Delaware</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>WCB Robotics India Pvt Ltd - Mechanical</t>
+          <t>Zeo - Product Management</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Mechanical</t>
+          <t>CSIS/IT</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>32500</v>
+        <v>50000</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Delaware</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>WILP - ADAS /  Autonomous Vehicle, Hyderabad</t>
+          <t>Zyduslife - Quant Analyst</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Mechanical</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr"/>
+          <t>Health Care</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>50000</v>
+      </c>
       <c r="D147" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>WILP - Additive Manufacturing, Hyderabad</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Mechanical</t>
-        </is>
-      </c>
-      <c r="C148" t="n">
-        <v>0</v>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>WILP - Electric and Hybrid Lab</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Mechanical</t>
-        </is>
-      </c>
-      <c r="C149" t="n">
-        <v>0</v>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>WILP- Intelligent systems Lab</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>Mechanical</t>
-        </is>
-      </c>
-      <c r="C150" t="n">
-        <v>0</v>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>WILP, Hyderabad</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>CSIS/IT</t>
-        </is>
-      </c>
-      <c r="C151" t="n">
-        <v>0</v>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>WILP-New Automotive Competency Centre Chennai (ACC)</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>Mechanical</t>
-        </is>
-      </c>
-      <c r="C152" t="n">
-        <v>0</v>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>Chennai</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>WILP-Vehicle security penetration testing facility in collaboration with Bosch</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>Mechanical</t>
-        </is>
-      </c>
-      <c r="C153" t="n">
-        <v>0</v>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>WizLearnr</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>CSIS/IT</t>
-        </is>
-      </c>
-      <c r="C154" t="n">
-        <v>0</v>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>Zeo - Product Content</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>CSIS/IT</t>
-        </is>
-      </c>
-      <c r="C155" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>Delaware</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>Zeo - Product Growth</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>CSIS/IT</t>
-        </is>
-      </c>
-      <c r="C156" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>Delaware</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>Zeo - Product Management</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>CSIS/IT</t>
-        </is>
-      </c>
-      <c r="C157" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>Delaware</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>Zyduslife - Quant Analyst</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>Health Care</t>
-        </is>
-      </c>
-      <c r="C158" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D158" t="inlineStr">
         <is>
           <t>Mumbai</t>
         </is>

</xml_diff>